<commit_message>
made some changes in code
</commit_message>
<xml_diff>
--- a/LinkAutomation/Reources/links.xlsx
+++ b/LinkAutomation/Reources/links.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="9732" windowWidth="24000" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="7248" windowWidth="19200" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -24,36 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>https://test.usc.jhancock.com/FIM/sps/uscfed/usc/self/account/create/validate?usc.confirmation.code=Te9lmMNbzZp%2F5caJ%2BhBc3qciFX5zdXRhcGEzMDEwMjAxOQ%3D%3D&amp;isambrand=johnhancockinsurance</t>
-  </si>
-  <si>
-    <t>uid</t>
-  </si>
-  <si>
-    <t>jjj</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>kljkljk</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/14013644/hosting-a-maven-repository-on-github</t>
+  </si>
+  <si>
+    <t>https://test.usc.jhancock.com/FIM/sps/uscfed/usc/self/account/create/validate?usc.confirmation.code=4INpIbVoHxSsTBmX4%2Bl2%2BNvYRZRzdXRhcGEzNjA4MTk%3D&amp;isambrand=johnhancockinsurance</t>
+  </si>
+  <si>
+    <t>https://test.usc.jhancock.com/FIM/sps/uscfed/usc/self/account/create/validate?usc.confirmation.code=QcID4SmBTkuHx8agV5mhLfXZDKdzdXRhcGEzNzA4MTk%3D&amp;isambrand=johnhancockinsurance</t>
   </si>
   <si>
     <t>Not Success</t>
   </si>
   <si>
-    <t>jhjkh</t>
-  </si>
-  <si>
-    <t>8jjg</t>
-  </si>
-  <si>
-    <t>https://test.usc.jhancock.com/FIM/sps/uscfed/usc/self/account/create/validate?usc.confirmation.code=4INpIbVoHxSsTBmX4%2Bl2%2BNvYRZRzdXRhcGEzNjA4MTk%3D&amp;isambrand=johnhancockinsurance</t>
-  </si>
-  <si>
-    <t>https://test.usc.jhancock.com/FIM/sps/uscfed/usc/self/account/create/validate?usc.confirmation.code=QcID4SmBTkuHx8agV5mhLfXZDKdzdXRhcGEzNzA4MTk%3D&amp;isambrand=johnhancockinsurance</t>
-  </si>
-  <si>
-    <t>jgkj</t>
-  </si>
-  <si>
-    <t>hjgg</t>
+    <t>https://test.usc.jhancock.com/FIM/sps/uscfed/usc/self/account/create/validate?usc.confirmation.code=nyhaBkMaPEhf5AiRcjn9dfhvC1VzaHJ1dGhpMjAxMDIwMTk%3D&amp;isambrand=johnhancockinsurance</t>
   </si>
   <si>
     <t>Registration Successful</t>
@@ -64,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +67,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,11 +108,16 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -388,83 +399,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="77" zoomScaleNormal="77">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="176.0" collapsed="true"/>
+    <col min="1" max="2" style="3" width="8.88671875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" style="3" width="167.33203125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="3" width="72.5546875" collapsed="false"/>
+    <col min="5" max="10" style="3" width="8.88671875" collapsed="false"/>
+    <col min="11" max="11" customWidth="true" style="3" width="16.33203125" collapsed="false"/>
+    <col min="12" max="16384" style="3" width="8.88671875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1230</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>3</v>
+      <c r="K3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>45353</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row ht="14.4" r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>5365365</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="K5" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://u8890785.ct.sendgrid.net/wf/click?upn=AnCZ-2B1yl7xw0EvxQStf0z2Ki-2BPpTHO279nZo-2B48EOS7h9OpxW5dM5Dcbm6Xs0Ois1mrL4vDCXSTuBT3h8UmyBLQGXFueX-2FbR7882650uyVza-2BznMZkZMfae2GfPrDQZrOtj9NrgjPYY6f-2BR8APd21ji0ZrjStyLc1OrgeL34mIKOVXbSGSmH2uBXu-2FBRBbnT9yyp1am5A7SQGVDDHbOTAgTl3FUPxG-2BbdWJPN-2FNyk0tgVOuJ88cA65GSoApbh1iJhnVbcruozioy2lLInG3g-2BQ-3D-3D_nTAKmd9rrJnwF9RD-2FR88IPs5beHkQoDWFVEIckd6-2FwYFm9z7ZYfhcLlLC9sQUfE9Se21ckzuxoqBoqoHlZ-2FaTGmCxUJHP2sEECZd5ga2sfB3bmt3MciKpVrNxvXWrh-2FB2i3UbWT5GqUBsPmtVatLvez1y9chE1qWBVLOnbhUAEC9Vg570Vre-2BZ5LLCUirl5aw4qeXnCc9QCgT0VieBgAhL2Y3xkJuTetDX-2FA3wV-2BgGRVecvhEe3ti0epK9niizlL" r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId1" ref="C2"/>
     <hyperlink display="https://u8890785.ct.sendgrid.net/wf/click?upn=AnCZ-2B1yl7xw0EvxQStf0z2Ki-2BPpTHO279nZo-2B48EOS7h9OpxW5dM5Dcbm6Xs0Ois1mrL4vDCXSTuBT3h8UmyBLQGXFueX-2FbR7882650uyVza-2BznMZkZMfae2GfPrDQZrogicFWI27-2F02J9awR7sQCHv65rOpOwM9FIWEe1OmDIV-2BJzztU7-2BjxKL1bWJjHPE-2Be-2Fs9lJ4K7gx0Z-2BgSgM30fg9-2BgWigl-2BgVSWU7PJ13TkGXvxNjmreTNAfZNyCJPy1k_nTAKmd9rrJnwF9RD-2FR88IB3aoZFlfDZvPt8SnHo4T15fLmtQVt82I9w87lMfEEPZMAGjIglfh5oWl1QmLf-2FABV68knp73gPna5X26kw02tkofZz5Vv8toh1figxevIZ87bgJUJxZ9yqiSTgtNpcNIPFCPjb9RpfQgVG4ZVSjVYDyD93B-2BZnVZ3hmaVfyW-2BmDNWUujm3jwY8QYGrsc3QsW5gsk2jpuuWOXU21hQ-2FGLLA6Wo-2Ftgz35Hi4wBcwUr8-2Fo" r:id="rId2" ref="C3"/>
     <hyperlink display="https://u8890785.ct.sendgrid.net/wf/click?upn=AnCZ-2B1yl7xw0EvxQStf0z2Ki-2BPpTHO279nZo-2B48EOS7h9OpxW5dM5Dcbm6Xs0Ois1mrL4vDCXSTuBT3h8UmyBLQGXFueX-2FbR7882650uyVza-2BznMZkZMfae2GfPrDQZr2rB6uOson8A9Vv4l9uP0HbuBiR-2F79jO5-2FrHbOhNgivd-2FkGiKFIQSjhNdzUuiRW0vBAatwEzjVCOxpW-2FbZuqV4XI-2F4YQt2LRKFs02U6GiQe-2FijRtnF3-2FEb3PjRC8pAjsQ_nTAKmd9rrJnwF9RD-2FR88IJhby8LLnGju1vm-2F1NmOuzEd4g72CzKFoh4-2Fmc113MOma8V2Cg4K3TXoFjaF1g-2Btw4twNLBekTvvwm-2BW3Uv0vX6RSncy3K-2Fa3WWnjjOcDoH28S-2FmPbEiEaVzr22fOX-2BVOmxIVC5CWUi7e6s6RzrUV27xZZyGOIK7P52KKtESufwgj5cjRQrfG-2B9saTMZ9C0WpuBNKhuD8ZKfW4PABCHOZjH9gKwoBuzgYl6OSNbdrSwf" r:id="rId3" ref="C4"/>
+    <hyperlink display="https://u8890785.ct.sendgrid.net/wf/click?upn=AnCZ-2B1yl7xw0EvxQStf0z2Ki-2BPpTHO279nZo-2B48EOS7h9OpxW5dM5Dcbm6Xs0Ois1mrL4vDCXSTuBT3h8UmyBLQGXFueX-2FbR7882650uyVza-2BznMZkZMfae2GfPrDQZrzpoXKFgjC7F-2FfQkJ8qWhzu-2BLToeYxrHKau9d3PiIwXzuWtDbdy37f0Rjk6wtwu9Y-2FG6SfowmL71ZZujMIQn7pj7JtpQZa3gHEWYOeDsB6WvLhWfl0MWjzR9UhuGxTodm_27UR-2FR4-2B-2FqDee8j9kcbWaPfZ3CBxd-2BVeC2lotzQvFqyONxv9YTmtPyxGYjmuhIWsFRF72keJRgfr7Ky5R1BFn-2BBzj9inLlDvuHtE9Prcu-2FVp9BfE-2Fk5vxNhOfq3rJHSWXNKjnA57tx8LV0UpulWZAIgNKjXJyLWfJ97i0ilNLWVcvPIesBOzc-2BKnAnMiVgGWUuEhhNL3b-2F3NR3nqf7mXfdeqr7r4S1KTweGuKvhmxsvKjhk7X-2F-2FzVOPQWCyHbvt-2B" r:id="rId4" ref="C5"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes in pom.xml and update
</commit_message>
<xml_diff>
--- a/LinkAutomation/Reources/links.xlsx
+++ b/LinkAutomation/Reources/links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>abc</t>
   </si>
@@ -407,12 +407,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" style="3" width="8.88671875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="3" width="167.33203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="3" width="72.5546875" collapsed="false"/>
-    <col min="5" max="10" style="3" width="8.88671875" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="3" width="16.33203125" collapsed="false"/>
-    <col min="12" max="16384" style="3" width="8.88671875" collapsed="false"/>
+    <col min="1" max="2" style="3" width="8.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="167.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="72.5546875" collapsed="true"/>
+    <col min="5" max="10" style="3" width="8.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="3" width="16.33203125" collapsed="true"/>
+    <col min="12" max="16384" style="3" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>